<commit_message>
locator master fetch changes, login ui changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C291825\OneDrive - Thomson Reuters Incorporated\Documents\UiPath\BulkClientCreationGo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C291825\OneDrive - Thomson Reuters Incorporated\Documents\UiPath\TR_Bulk_ClientCreation_GO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195C7EFB-4889-4857-9DF3-69224917FDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6954BF81-4BE2-45F1-99C2-83D4F22825C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1694,7 +1694,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>

</xml_diff>